<commit_message>
add prodi in mhs
</commit_message>
<xml_diff>
--- a/public/assets/dist/format/mahasiswa_simple.xlsx
+++ b/public/assets/dist/format/mahasiswa_simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/undipmac/Documents/WEBAPP/CODEIGNITER/ujianundip/public/assets/dist/format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F71E0390-6C67-0947-AE49-876B9849E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1CD22A-43A3-E443-9F48-52290BA52C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>L/P</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>NO BILLKEY</t>
+  </si>
+  <si>
+    <t>PRODI</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -453,10 +456,11 @@
     <col min="6" max="6" width="7" style="3" customWidth="1"/>
     <col min="7" max="7" width="27.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="36.6640625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="2"/>
+    <col min="9" max="9" width="45" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -481,22 +485,25 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="7"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="7"/>
       <c r="F3" s="4"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="7"/>

</xml_diff>

<commit_message>
fix(mhs): memperbaiki import mhs ditambah gel dan tahun
</commit_message>
<xml_diff>
--- a/public/assets/dist/format/mahasiswa_simple.xlsx
+++ b/public/assets/dist/format/mahasiswa_simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/undipmac/Documents/WEBAPP/CODEIGNITER/ujianundip/public/assets/dist/format/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/the-black-pearl/Repositories/ujianundip/public/assets/dist/format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1CD22A-43A3-E443-9F48-52290BA52C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724A8525-5ADA-D948-97DA-6523658FBC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>L/P</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>PRODI</t>
+  </si>
+  <si>
+    <t>GEL</t>
+  </si>
+  <si>
+    <t>TAHUN</t>
   </si>
 </sst>
 </file>
@@ -114,18 +120,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -133,13 +133,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -441,74 +438,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="15.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="45" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="2"/>
+    <col min="1" max="2" width="15.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="7" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="45" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="7"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
+    <row r="2" spans="1:11">
+      <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
+    <row r="3" spans="1:11">
+      <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
+    <row r="4" spans="1:11">
+      <c r="G4" s="3"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -526,8 +517,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -545,8 +535,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>